<commit_message>
spring file upload - register, system
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\학원 프로젝트\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\학원프로젝트\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA42EBF-D5CA-4096-9601-6A2F4E9A0B22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CF2A81-3C29-445F-8920-23EE5897ACAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5452EA78-F9CF-4924-AB73-13A308B8C969}"/>
+    <workbookView xWindow="396" yWindow="300" windowWidth="11724" windowHeight="8964" xr2:uid="{5452EA78-F9CF-4924-AB73-13A308B8C969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="203">
   <si>
     <t>팀(논리)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -873,7 +873,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -905,6 +905,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1223,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F199E4-88F1-478C-9FE5-67B2B014272F}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1629,6 +1632,12 @@
       <c r="D11" s="7">
         <v>2</v>
       </c>
+      <c r="E11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="I11" s="2" t="s">
         <v>51</v>
       </c>

</xml_diff>